<commit_message>
transfer to clf org
</commit_message>
<xml_diff>
--- a/Holbrook actionables.xlsx
+++ b/Holbrook actionables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilyfang/Desktop/clf/healthscore_automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EC1F21-1E3A-C240-9494-5C48D5056FFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E4DCE4-7BD4-214E-B5C0-D52756E30258}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -582,7 +582,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>